<commit_message>
agent integration and initial UI created
</commit_message>
<xml_diff>
--- a/Sample_Evaluation.xlsx
+++ b/Sample_Evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b3555fed9142bb87/Desktop/UD AI Agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{B4FDBFFD-88CD-435D-9CAC-5E135DEE9DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="14_{B4FDBFFD-88CD-435D-9CAC-5E135DEE9DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AD7BB40-71A4-4B45-B4AA-1905CE2E7530}"/>
   <bookViews>
-    <workbookView xWindow="22450" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{BE44486A-45EF-41AC-A974-A3ED3817167D}"/>
+    <workbookView minimized="1" xWindow="3000" yWindow="3000" windowWidth="16920" windowHeight="10450" xr2:uid="{BE44486A-45EF-41AC-A974-A3ED3817167D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <t>Sequencing Score (5-correct, 1-incorrect)</t>
   </si>
   <si>
-    <t>Are birds green? ( want to see no results for this )</t>
+    <t>Are birds green?</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>